<commit_message>
Add pie charts legend
</commit_message>
<xml_diff>
--- a/regions_data/Ciepłownictwo/pie_chart_data/1_Produkcja ciepła wg paliw.xlsx
+++ b/regions_data/Ciepłownictwo/pie_chart_data/1_Produkcja ciepła wg paliw.xlsx
@@ -22,7 +22,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="123">
   <si>
-    <t xml:space="preserve">Tabela</t>
+    <t xml:space="preserve">Nazwa wycinka</t>
   </si>
   <si>
     <t xml:space="preserve">Dolnośląskie</t>
@@ -488,146 +488,144 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Q10"/>
+  <dimension ref="B1:R10"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D16" activeCellId="0" sqref="D16"/>
+      <selection pane="topLeft" activeCell="B17" activeCellId="0" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.4795918367347"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.1326530612245"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.7704081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="B1" s="0" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="C1" s="0" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="D1" s="0" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="E1" s="0" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="F1" s="0" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="G1" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="H1" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="0" t="s">
+      <c r="I1" s="0" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="0" t="s">
+      <c r="J1" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="0" t="s">
+      <c r="K1" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="0" t="s">
+      <c r="L1" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="0" t="s">
+      <c r="M1" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="0" t="s">
+      <c r="N1" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="0" t="s">
+      <c r="O1" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="0" t="s">
+      <c r="P1" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="0" t="s">
+      <c r="Q1" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="0" t="s">
+      <c r="R1" s="0" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="B2" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="C2" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="D2" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="E2" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="E2" s="0" t="s">
+      <c r="F2" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="F2" s="0" t="s">
+      <c r="G2" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="G2" s="0" t="s">
+      <c r="H2" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="H2" s="0" t="s">
+      <c r="I2" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="I2" s="0" t="s">
+      <c r="J2" s="0" t="s">
         <v>25</v>
       </c>
-      <c r="J2" s="0" t="s">
+      <c r="K2" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="K2" s="0" t="s">
+      <c r="L2" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="L2" s="0" t="s">
+      <c r="M2" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="M2" s="0" t="s">
+      <c r="N2" s="0" t="s">
         <v>29</v>
       </c>
-      <c r="N2" s="0" t="s">
+      <c r="O2" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="O2" s="0" t="s">
+      <c r="P2" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="P2" s="0" t="s">
+      <c r="Q2" s="0" t="s">
         <v>32</v>
       </c>
-      <c r="Q2" s="0" t="s">
+      <c r="R2" s="0" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="B3" s="0" t="s">
         <v>34</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="C3" s="0" t="s">
         <v>35</v>
       </c>
-      <c r="C3" s="0" t="s">
-        <v>36</v>
-      </c>
       <c r="D3" s="0" t="s">
         <v>36</v>
       </c>
       <c r="E3" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="F3" s="0" t="s">
         <v>37</v>
       </c>
-      <c r="F3" s="0" t="s">
+      <c r="G3" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="G3" s="0" t="s">
-        <v>36</v>
-      </c>
       <c r="H3" s="0" t="s">
         <v>36</v>
       </c>
@@ -653,78 +651,78 @@
         <v>36</v>
       </c>
       <c r="P3" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q3" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="Q3" s="0" t="s">
+      <c r="R3" s="0" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="B4" s="0" t="s">
         <v>40</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="C4" s="0" t="s">
         <v>41</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="D4" s="0" t="s">
         <v>42</v>
       </c>
-      <c r="D4" s="0" t="s">
-        <v>36</v>
-      </c>
       <c r="E4" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="F4" s="0" t="s">
         <v>43</v>
       </c>
-      <c r="F4" s="0" t="s">
+      <c r="G4" s="0" t="s">
         <v>44</v>
       </c>
-      <c r="G4" s="0" t="s">
+      <c r="H4" s="0" t="s">
         <v>45</v>
       </c>
-      <c r="H4" s="0" t="s">
+      <c r="I4" s="0" t="s">
         <v>46</v>
       </c>
-      <c r="I4" s="0" t="s">
+      <c r="J4" s="0" t="s">
         <v>47</v>
       </c>
-      <c r="J4" s="0" t="s">
+      <c r="K4" s="0" t="s">
         <v>48</v>
       </c>
-      <c r="K4" s="0" t="s">
+      <c r="L4" s="0" t="s">
         <v>49</v>
       </c>
-      <c r="L4" s="0" t="s">
+      <c r="M4" s="0" t="s">
         <v>50</v>
       </c>
-      <c r="M4" s="0" t="s">
+      <c r="N4" s="0" t="s">
         <v>51</v>
       </c>
-      <c r="N4" s="0" t="s">
+      <c r="O4" s="0" t="s">
         <v>52</v>
       </c>
-      <c r="O4" s="0" t="s">
+      <c r="P4" s="0" t="s">
         <v>53</v>
       </c>
-      <c r="P4" s="0" t="s">
+      <c r="Q4" s="0" t="s">
         <v>54</v>
       </c>
-      <c r="Q4" s="0" t="s">
+      <c r="R4" s="0" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="B5" s="0" t="s">
         <v>56</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="C5" s="0" t="s">
         <v>57</v>
       </c>
-      <c r="C5" s="0" t="s">
+      <c r="D5" s="0" t="s">
         <v>58</v>
       </c>
-      <c r="D5" s="0" t="s">
-        <v>36</v>
-      </c>
       <c r="E5" s="0" t="s">
         <v>36</v>
       </c>
@@ -732,14 +730,14 @@
         <v>36</v>
       </c>
       <c r="G5" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="H5" s="0" t="s">
         <v>59</v>
       </c>
-      <c r="H5" s="0" t="s">
+      <c r="I5" s="0" t="s">
         <v>60</v>
       </c>
-      <c r="I5" s="0" t="s">
-        <v>36</v>
-      </c>
       <c r="J5" s="0" t="s">
         <v>36</v>
       </c>
@@ -747,14 +745,14 @@
         <v>36</v>
       </c>
       <c r="L5" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="M5" s="0" t="s">
         <v>61</v>
       </c>
-      <c r="M5" s="0" t="s">
+      <c r="N5" s="0" t="s">
         <v>62</v>
       </c>
-      <c r="N5" s="0" t="s">
-        <v>36</v>
-      </c>
       <c r="O5" s="0" t="s">
         <v>36</v>
       </c>
@@ -762,93 +760,93 @@
         <v>36</v>
       </c>
       <c r="Q5" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="R5" s="0" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="B6" s="0" t="s">
         <v>63</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="C6" s="0" t="s">
         <v>64</v>
       </c>
-      <c r="C6" s="0" t="s">
+      <c r="D6" s="0" t="s">
         <v>65</v>
       </c>
-      <c r="D6" s="0" t="s">
+      <c r="E6" s="0" t="s">
         <v>66</v>
       </c>
-      <c r="E6" s="0" t="s">
+      <c r="F6" s="0" t="s">
         <v>67</v>
       </c>
-      <c r="F6" s="0" t="s">
+      <c r="G6" s="0" t="s">
         <v>68</v>
       </c>
-      <c r="G6" s="0" t="s">
+      <c r="H6" s="0" t="s">
         <v>69</v>
       </c>
-      <c r="H6" s="0" t="s">
+      <c r="I6" s="0" t="s">
         <v>70</v>
       </c>
-      <c r="I6" s="0" t="s">
+      <c r="J6" s="0" t="s">
         <v>71</v>
       </c>
-      <c r="J6" s="0" t="s">
+      <c r="K6" s="0" t="s">
         <v>72</v>
       </c>
-      <c r="K6" s="0" t="s">
+      <c r="L6" s="0" t="s">
         <v>73</v>
       </c>
-      <c r="L6" s="0" t="s">
+      <c r="M6" s="0" t="s">
         <v>74</v>
       </c>
-      <c r="M6" s="0" t="s">
+      <c r="N6" s="0" t="s">
         <v>75</v>
       </c>
-      <c r="N6" s="0" t="s">
+      <c r="O6" s="0" t="s">
         <v>76</v>
       </c>
-      <c r="O6" s="0" t="s">
+      <c r="P6" s="0" t="s">
         <v>77</v>
       </c>
-      <c r="P6" s="0" t="s">
+      <c r="Q6" s="0" t="s">
         <v>78</v>
       </c>
-      <c r="Q6" s="0" t="s">
+      <c r="R6" s="0" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+      <c r="B7" s="0" t="s">
         <v>80</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="C7" s="0" t="s">
         <v>81</v>
       </c>
-      <c r="C7" s="0" t="s">
-        <v>36</v>
-      </c>
       <c r="D7" s="0" t="s">
         <v>36</v>
       </c>
       <c r="E7" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="F7" s="0" t="s">
         <v>82</v>
       </c>
-      <c r="F7" s="0" t="s">
-        <v>36</v>
-      </c>
       <c r="G7" s="0" t="s">
         <v>36</v>
       </c>
       <c r="H7" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="I7" s="0" t="s">
         <v>83</v>
       </c>
-      <c r="I7" s="0" t="s">
+      <c r="J7" s="0" t="s">
         <v>84</v>
       </c>
-      <c r="J7" s="0" t="s">
-        <v>36</v>
-      </c>
       <c r="K7" s="0" t="s">
         <v>36</v>
       </c>
@@ -865,75 +863,75 @@
         <v>36</v>
       </c>
       <c r="P7" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q7" s="0" t="s">
         <v>85</v>
       </c>
-      <c r="Q7" s="0" t="s">
+      <c r="R7" s="0" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+      <c r="B8" s="0" t="s">
         <v>87</v>
       </c>
-      <c r="B8" s="0" t="s">
+      <c r="C8" s="0" t="s">
         <v>88</v>
       </c>
-      <c r="C8" s="0" t="s">
+      <c r="D8" s="0" t="s">
         <v>89</v>
       </c>
-      <c r="D8" s="0" t="s">
+      <c r="E8" s="0" t="s">
         <v>90</v>
       </c>
-      <c r="E8" s="0" t="s">
+      <c r="F8" s="0" t="s">
         <v>91</v>
       </c>
-      <c r="F8" s="0" t="s">
+      <c r="G8" s="0" t="s">
         <v>92</v>
       </c>
-      <c r="G8" s="0" t="s">
+      <c r="H8" s="0" t="s">
         <v>93</v>
       </c>
-      <c r="H8" s="0" t="s">
+      <c r="I8" s="0" t="s">
         <v>94</v>
       </c>
-      <c r="I8" s="0" t="s">
+      <c r="J8" s="0" t="s">
         <v>95</v>
       </c>
-      <c r="J8" s="0" t="s">
+      <c r="K8" s="0" t="s">
         <v>96</v>
       </c>
-      <c r="K8" s="0" t="s">
+      <c r="L8" s="0" t="s">
         <v>97</v>
       </c>
-      <c r="L8" s="0" t="s">
+      <c r="M8" s="0" t="s">
         <v>98</v>
       </c>
-      <c r="M8" s="0" t="s">
+      <c r="N8" s="0" t="s">
         <v>99</v>
       </c>
-      <c r="N8" s="0" t="s">
+      <c r="O8" s="0" t="s">
         <v>100</v>
       </c>
-      <c r="O8" s="0" t="s">
+      <c r="P8" s="0" t="s">
         <v>101</v>
       </c>
-      <c r="P8" s="0" t="s">
+      <c r="Q8" s="0" t="s">
         <v>102</v>
       </c>
-      <c r="Q8" s="0" t="s">
+      <c r="R8" s="0" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+      <c r="B9" s="0" t="s">
         <v>104</v>
       </c>
-      <c r="B9" s="0" t="s">
+      <c r="C9" s="0" t="s">
         <v>105</v>
       </c>
-      <c r="C9" s="0" t="s">
-        <v>36</v>
-      </c>
       <c r="D9" s="0" t="s">
         <v>36</v>
       </c>
@@ -941,49 +939,49 @@
         <v>36</v>
       </c>
       <c r="F9" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="G9" s="0" t="s">
         <v>106</v>
       </c>
-      <c r="G9" s="0" t="s">
+      <c r="H9" s="0" t="s">
         <v>107</v>
       </c>
-      <c r="H9" s="0" t="s">
+      <c r="I9" s="0" t="s">
         <v>108</v>
       </c>
-      <c r="I9" s="0" t="s">
+      <c r="J9" s="0" t="s">
         <v>109</v>
       </c>
-      <c r="J9" s="0" t="s">
+      <c r="K9" s="0" t="s">
         <v>110</v>
       </c>
-      <c r="K9" s="0" t="s">
-        <v>36</v>
-      </c>
       <c r="L9" s="0" t="s">
         <v>36</v>
       </c>
       <c r="M9" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="N9" s="0" t="s">
         <v>111</v>
       </c>
-      <c r="N9" s="0" t="s">
-        <v>36</v>
-      </c>
       <c r="O9" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="P9" s="0" t="s">
         <v>112</v>
       </c>
-      <c r="P9" s="0" t="s">
-        <v>36</v>
-      </c>
       <c r="Q9" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="R9" s="0" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
+      <c r="B10" s="0" t="s">
         <v>114</v>
       </c>
-      <c r="B10" s="0" t="s">
-        <v>36</v>
-      </c>
       <c r="C10" s="0" t="s">
         <v>36</v>
       </c>
@@ -994,39 +992,42 @@
         <v>36</v>
       </c>
       <c r="F10" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="G10" s="0" t="s">
         <v>115</v>
       </c>
-      <c r="G10" s="0" t="s">
+      <c r="H10" s="0" t="s">
         <v>116</v>
       </c>
-      <c r="H10" s="0" t="s">
+      <c r="I10" s="0" t="s">
         <v>117</v>
       </c>
-      <c r="I10" s="0" t="s">
-        <v>36</v>
-      </c>
       <c r="J10" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="K10" s="0" t="s">
         <v>118</v>
       </c>
-      <c r="K10" s="0" t="s">
-        <v>36</v>
-      </c>
       <c r="L10" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="M10" s="0" t="s">
         <v>119</v>
       </c>
-      <c r="M10" s="0" t="s">
+      <c r="N10" s="0" t="s">
         <v>120</v>
       </c>
-      <c r="N10" s="0" t="s">
-        <v>36</v>
-      </c>
       <c r="O10" s="0" t="s">
         <v>36</v>
       </c>
       <c r="P10" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q10" s="0" t="s">
         <v>121</v>
       </c>
-      <c r="Q10" s="0" t="s">
+      <c r="R10" s="0" t="s">
         <v>122</v>
       </c>
     </row>

</xml_diff>